<commit_message>
Update Customers database table
</commit_message>
<xml_diff>
--- a/raw_data/customers_db.xlsx
+++ b/raw_data/customers_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alisa/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77342BF-B982-E049-BD65-50B2D21959BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C84D193-1545-42D5-8FF4-8416E8060625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="5140" windowWidth="23260" windowHeight="12460" xr2:uid="{55055081-DE6E-4B45-951F-D4AB37DE9E6F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55055081-DE6E-4B45-951F-D4AB37DE9E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>customer_id</t>
   </si>
@@ -56,127 +59,34 @@
     <t>John</t>
   </si>
   <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>jwick1</t>
-  </si>
-  <si>
     <t>account_value</t>
   </si>
   <si>
     <t>cups_bought</t>
   </si>
   <si>
-    <t>Carroll</t>
-  </si>
-  <si>
-    <t>Nick</t>
-  </si>
-  <si>
-    <t>ncarroll1</t>
-  </si>
-  <si>
-    <t>Jenny</t>
-  </si>
-  <si>
-    <t>password1</t>
-  </si>
-  <si>
-    <t>password2</t>
-  </si>
-  <si>
-    <t>password3</t>
-  </si>
-  <si>
-    <t>Miftah</t>
-  </si>
-  <si>
-    <t>Wafiakmal</t>
-  </si>
-  <si>
-    <t>wafi1</t>
-  </si>
-  <si>
-    <t>password4</t>
-  </si>
-  <si>
-    <t>Alisa</t>
-  </si>
-  <si>
-    <t>Tian</t>
-  </si>
-  <si>
-    <t>atian1</t>
-  </si>
-  <si>
-    <t>password5</t>
-  </si>
-  <si>
-    <t>Shen</t>
-  </si>
-  <si>
-    <t>jshen1</t>
-  </si>
-  <si>
     <t>cup_rental</t>
   </si>
   <si>
-    <t>Lin</t>
-  </si>
-  <si>
-    <t>Abby2</t>
-  </si>
-  <si>
-    <t>Snow</t>
-  </si>
-  <si>
-    <t>Wang</t>
-  </si>
-  <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t>lIA</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>wafi2</t>
-  </si>
-  <si>
-    <t>password6</t>
-  </si>
-  <si>
-    <t>atian2</t>
-  </si>
-  <si>
-    <t>password7</t>
-  </si>
-  <si>
-    <t>wafi3</t>
-  </si>
-  <si>
-    <t>password8</t>
-  </si>
-  <si>
-    <t>atian3</t>
-  </si>
-  <si>
-    <t>password9</t>
-  </si>
-  <si>
-    <t>wafi4</t>
-  </si>
-  <si>
-    <t>password10</t>
+    <t>McFly</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Corleone</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Durden</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>McClane</t>
   </si>
 </sst>
 </file>
@@ -186,16 +96,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -538,20 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617DB90-6D3E-464D-87D2-F756CC04DABA}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
     <col min="5" max="10" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -565,25 +469,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>14045</v>
       </c>
@@ -602,22 +500,16 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>14046</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>44901</v>
@@ -628,22 +520,16 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>14047</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>44846</v>
@@ -657,22 +543,16 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>14048</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>44849</v>
@@ -683,22 +563,16 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14049</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1">
         <v>44834</v>
@@ -712,145 +586,8 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>14050</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44846</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>14052</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44849</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>1.3</v>
-      </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>14054</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1">
-        <v>44834</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>1.6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>14056</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44846</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10">
-        <v>1.9</v>
-      </c>
-      <c r="I10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>14057</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44839</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" t="s">
-        <v>47</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>